<commit_message>
Added R scripts and updated .gitignore
</commit_message>
<xml_diff>
--- a/Data/VolunteersV02.xlsx
+++ b/Data/VolunteersV02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iowa-my.sharepoint.com/personal/martie_uiowa_edu/Documents/Work/ISRP/Project3/Wristband/WristBandProject/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{7C341129-3D96-3C49-AA99-7D534F77425B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D89E7E5-3217-1045-8665-17C65B4A9B24}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{7C341129-3D96-3C49-AA99-7D534F77425B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B3093CF-2CEE-40CC-830C-E1A24274903D}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{59579006-5D5C-E441-B1BF-CC0305387B64}"/>
+    <workbookView xWindow="7160" yWindow="290" windowWidth="28820" windowHeight="20150" xr2:uid="{59579006-5D5C-E441-B1BF-CC0305387B64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4848,7 +4848,7 @@
         </row>
         <row r="10">
           <cell r="A10" t="str">
-            <v>wb.Ta.h</v>
+            <v>wb.Ya.h</v>
           </cell>
           <cell r="B10">
             <v>3.3166666666656965</v>
@@ -5426,7 +5426,7 @@
             <v>0.49484795474277515</v>
           </cell>
           <cell r="R11">
-            <v>3.9276950941239304</v>
+            <v>0.30782942391693102</v>
           </cell>
           <cell r="S11">
             <v>0.89931613185096881</v>
@@ -5447,7 +5447,7 @@
             <v>5.7579624561924564E-3</v>
           </cell>
           <cell r="Y11">
-            <v>1.515384888299935E-3</v>
+            <v>2.3884275254398978E-2</v>
           </cell>
           <cell r="Z11">
             <v>6.6115253436070776E-2</v>
@@ -5456,7 +5456,7 @@
             <v>0.12716705873436737</v>
           </cell>
           <cell r="AB11">
-            <v>5.5705370292952257E-2</v>
+            <v>4.608829279023581E-2</v>
           </cell>
           <cell r="AC11">
             <v>0.64977302374869217</v>
@@ -7806,8 +7806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45080374-5481-CA42-8BD4-A17D4E91A9C5}">
   <dimension ref="A1:FS14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="BW1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="BY1" sqref="BY1:BY14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -14133,7 +14133,7 @@
     <row r="10" spans="1:175" x14ac:dyDescent="0.4">
       <c r="A10" t="str">
         <f>'[1]Datafor R'!A10</f>
-        <v>wb.Ta.h</v>
+        <v>wb.Ya.h</v>
       </c>
       <c r="B10">
         <f>'[1]Datafor R'!B10</f>
@@ -14903,7 +14903,7 @@
       </c>
       <c r="R11">
         <f>'[1]Datafor R'!R11</f>
-        <v>3.9276950941239304</v>
+        <v>0.30782942391693102</v>
       </c>
       <c r="S11">
         <f>'[1]Datafor R'!S11</f>
@@ -14931,7 +14931,7 @@
       </c>
       <c r="Y11">
         <f>'[1]Datafor R'!Y11</f>
-        <v>1.515384888299935E-3</v>
+        <v>2.3884275254398978E-2</v>
       </c>
       <c r="Z11">
         <f>'[1]Datafor R'!Z11</f>
@@ -14943,7 +14943,7 @@
       </c>
       <c r="AB11">
         <f>'[1]Datafor R'!AB11</f>
-        <v>5.5705370292952257E-2</v>
+        <v>4.608829279023581E-2</v>
       </c>
       <c r="AC11">
         <f>'[1]Datafor R'!AC11</f>

</xml_diff>